<commit_message>
added info for sheets that were used in search. Need to clean up formatting.
</commit_message>
<xml_diff>
--- a/PyCharm_Oligo/AZ Oligos.xlsx
+++ b/PyCharm_Oligo/AZ Oligos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="517">
   <si>
     <t>AZ26</t>
   </si>
@@ -1943,12 +1943,15 @@
   <si>
     <t>60 bp downstream</t>
   </si>
+  <si>
+    <t>Oligo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2205,6 +2208,12 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -3867,7 +3876,7 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4040,6 +4049,7 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1575">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5983,8 +5993,8 @@
       <c r="B1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>12</v>
+      <c r="C1" s="96" t="s">
+        <v>516</v>
       </c>
       <c r="D1" s="47" t="s">
         <v>24</v>

</xml_diff>